<commit_message>
Timesheet Updated by Prathima
</commit_message>
<xml_diff>
--- a/Process/Timesheet/PTW-Timesheet .xlsx
+++ b/Process/Timesheet/PTW-Timesheet .xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\Aspire Intern - Workshop\Year 2022\Q1\To Trainees\Your Project Name\Process\Timesheet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{9472E262-E61E-41B3-A586-B0A8EE83E948}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{17FD74EB-D982-4002-B653-6AFFA4976974}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="23" activeTab="21" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -77,7 +77,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3274" uniqueCount="856">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3283" uniqueCount="859">
   <si>
     <t>Resource Name</t>
   </si>
@@ -2532,6 +2532,9 @@
     <t>Project Work for college</t>
   </si>
   <si>
+    <t>HTML refining</t>
+  </si>
+  <si>
     <t xml:space="preserve">Tutorial on Angular </t>
   </si>
   <si>
@@ -2550,7 +2553,7 @@
     <t>angular tutorial video</t>
   </si>
   <si>
-    <t>imp</t>
+    <t>implementing angular in vscode</t>
   </si>
   <si>
     <t>Refined layout pages</t>
@@ -2559,6 +2562,9 @@
     <t>Started working on angular</t>
   </si>
   <si>
+    <t>Model in angular refining</t>
+  </si>
+  <si>
     <t>Angular session</t>
   </si>
   <si>
@@ -2581,6 +2587,9 @@
   </si>
   <si>
     <t>Angular Tutorial</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Learned Angular </t>
   </si>
   <si>
     <t>Exploration on creating a component</t>
@@ -22825,25 +22834,45 @@
       <c r="B78" s="80" t="s">
         <v>749</v>
       </c>
-      <c r="C78" s="80"/>
-      <c r="D78" s="81"/>
-      <c r="E78" s="81"/>
-      <c r="F78" s="81"/>
+      <c r="C78" s="80" t="s">
+        <v>510</v>
+      </c>
+      <c r="D78" s="81">
+        <v>0.58333333333333337</v>
+      </c>
+      <c r="E78" s="81">
+        <v>0.625</v>
+      </c>
+      <c r="F78" s="81">
+        <f>E78-D78</f>
+        <v>4.166666666666663E-2</v>
+      </c>
       <c r="H78" s="83" t="s">
         <v>504</v>
       </c>
       <c r="I78" s="81">
         <f>SUMIFS(F77:F91, C77:C91,H78)</f>
-        <v>0</v>
+        <v>4.166666666666663E-2</v>
       </c>
     </row>
     <row r="79" spans="1:9">
       <c r="A79" s="99"/>
-      <c r="B79" s="80"/>
-      <c r="C79" s="80"/>
-      <c r="D79" s="81"/>
-      <c r="E79" s="81"/>
-      <c r="F79" s="81"/>
+      <c r="B79" s="80" t="s">
+        <v>755</v>
+      </c>
+      <c r="C79" s="80" t="s">
+        <v>504</v>
+      </c>
+      <c r="D79" s="81">
+        <v>0.64583333333333337</v>
+      </c>
+      <c r="E79" s="81">
+        <v>0.6875</v>
+      </c>
+      <c r="F79" s="81">
+        <f>E79-D79</f>
+        <v>4.166666666666663E-2</v>
+      </c>
       <c r="H79" s="83" t="s">
         <v>508</v>
       </c>
@@ -22864,7 +22893,7 @@
       </c>
       <c r="I80" s="81">
         <f>SUMIFS(F77:F91, C77:C91,H80)</f>
-        <v>0</v>
+        <v>4.166666666666663E-2</v>
       </c>
     </row>
     <row r="81" spans="1:9">
@@ -22924,7 +22953,7 @@
       </c>
       <c r="I84" s="79">
         <f>SUM(I78:I83)</f>
-        <v>0.12152777777777773</v>
+        <v>0.20486111111111099</v>
       </c>
     </row>
     <row r="85" spans="1:9">
@@ -23004,7 +23033,7 @@
     <row r="93" spans="1:9">
       <c r="A93" s="99"/>
       <c r="B93" s="80" t="s">
-        <v>755</v>
+        <v>756</v>
       </c>
       <c r="C93" s="80" t="s">
         <v>508</v>
@@ -23244,7 +23273,7 @@
     <row r="108" spans="1:9">
       <c r="A108" s="99"/>
       <c r="B108" s="80" t="s">
-        <v>756</v>
+        <v>757</v>
       </c>
       <c r="C108" s="80" t="s">
         <v>504</v>
@@ -23348,7 +23377,7 @@
     <row r="112" spans="1:9">
       <c r="A112" s="99"/>
       <c r="B112" s="80" t="s">
-        <v>757</v>
+        <v>758</v>
       </c>
       <c r="C112" s="80" t="s">
         <v>504</v>
@@ -23374,7 +23403,7 @@
     <row r="113" spans="1:9">
       <c r="A113" s="99"/>
       <c r="B113" s="80" t="s">
-        <v>758</v>
+        <v>759</v>
       </c>
       <c r="C113" s="80" t="s">
         <v>508</v>
@@ -23400,7 +23429,7 @@
     <row r="114" spans="1:9">
       <c r="A114" s="99"/>
       <c r="B114" s="80" t="s">
-        <v>759</v>
+        <v>760</v>
       </c>
       <c r="C114" s="80" t="s">
         <v>504</v>
@@ -23552,13 +23581,13 @@
       </c>
       <c r="I123" s="81">
         <f>SUMIFS(F122:F136, C122:C136,H123)</f>
-        <v>0.20833333333333337</v>
+        <v>0.25</v>
       </c>
     </row>
     <row r="124" spans="1:9">
       <c r="A124" s="99"/>
       <c r="B124" s="80" t="s">
-        <v>760</v>
+        <v>761</v>
       </c>
       <c r="C124" s="80" t="s">
         <v>510</v>
@@ -23578,33 +23607,33 @@
       </c>
       <c r="I124" s="81">
         <f>SUMIFS(F122:F136, C122:C136,H124)</f>
-        <v>4.1666666666666685E-2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="125" spans="1:9">
       <c r="A125" s="99"/>
       <c r="B125" s="80" t="s">
-        <v>761</v>
+        <v>762</v>
       </c>
       <c r="C125" s="80" t="s">
-        <v>508</v>
+        <v>504</v>
       </c>
       <c r="D125" s="81">
-        <v>0.47916666666666669</v>
+        <v>0.52083333333333337</v>
       </c>
       <c r="E125" s="81">
-        <v>0.52083333333333337</v>
+        <v>0.5625</v>
       </c>
       <c r="F125" s="81">
         <f>E125-D125</f>
-        <v>4.1666666666666685E-2</v>
+        <v>4.166666666666663E-2</v>
       </c>
       <c r="H125" s="83" t="s">
         <v>510</v>
       </c>
       <c r="I125" s="81">
         <f>SUMIFS(F122:F136, C122:C136,H125)</f>
-        <v>0.13541666666666669</v>
+        <v>2.430555555555558E-2</v>
       </c>
     </row>
     <row r="126" spans="1:9">
@@ -23616,14 +23645,14 @@
         <v>516</v>
       </c>
       <c r="D126" s="81">
-        <v>0.52083333333333337</v>
+        <v>0.5625</v>
       </c>
       <c r="E126" s="81">
-        <v>0.54166666666666663</v>
+        <v>0.58333333333333337</v>
       </c>
       <c r="F126" s="81">
         <f>E126-D126</f>
-        <v>2.0833333333333259E-2</v>
+        <v>2.083333333333337E-2</v>
       </c>
       <c r="H126" s="83" t="s">
         <v>513</v>
@@ -23636,20 +23665,20 @@
     <row r="127" spans="1:9">
       <c r="A127" s="99"/>
       <c r="B127" s="80" t="s">
-        <v>520</v>
+        <v>299</v>
       </c>
       <c r="C127" s="80" t="s">
-        <v>516</v>
+        <v>510</v>
       </c>
       <c r="D127" s="81">
-        <v>0.47222222222222227</v>
+        <v>0.59027777777777779</v>
       </c>
       <c r="E127" s="81">
         <v>0.47916666666666669</v>
       </c>
       <c r="F127" s="81">
         <f>E127-D127</f>
-        <v>6.9444444444444198E-3</v>
+        <v>-0.1111111111111111</v>
       </c>
       <c r="H127" s="83" t="s">
         <v>512</v>
@@ -23661,9 +23690,7 @@
     </row>
     <row r="128" spans="1:9">
       <c r="A128" s="99"/>
-      <c r="B128" s="80" t="s">
-        <v>521</v>
-      </c>
+      <c r="B128" s="80"/>
       <c r="C128" s="80" t="s">
         <v>516</v>
       </c>
@@ -23682,7 +23709,7 @@
       </c>
       <c r="I128" s="81">
         <f>SUMIFS(F122:F136, C122:C136,H128)</f>
-        <v>4.8611111111110994E-2</v>
+        <v>4.1666666666666685E-2</v>
       </c>
     </row>
     <row r="129" spans="1:9">
@@ -23708,7 +23735,7 @@
       </c>
       <c r="I129" s="79">
         <f>SUM(I123:I128)</f>
-        <v>0.43402777777777773</v>
+        <v>0.31597222222222227</v>
       </c>
     </row>
     <row r="130" spans="1:9">
@@ -24124,7 +24151,7 @@
     <row r="153" spans="1:9">
       <c r="A153" s="99"/>
       <c r="B153" s="80" t="s">
-        <v>762</v>
+        <v>763</v>
       </c>
       <c r="C153" s="80" t="s">
         <v>508</v>
@@ -24150,7 +24177,7 @@
     <row r="154" spans="1:9">
       <c r="A154" s="99"/>
       <c r="B154" s="80" t="s">
-        <v>763</v>
+        <v>764</v>
       </c>
       <c r="C154" s="80" t="s">
         <v>504</v>
@@ -24530,7 +24557,9 @@
     </row>
     <row r="3" spans="1:17">
       <c r="A3" s="99"/>
-      <c r="B3" s="80"/>
+      <c r="B3" s="80" t="s">
+        <v>765</v>
+      </c>
       <c r="C3" s="80" t="s">
         <v>504</v>
       </c>
@@ -24549,7 +24578,7 @@
       </c>
       <c r="I3" s="81">
         <f>SUMIFS(F2:F16, C2:C16,H3)</f>
-        <v>2.7777777777777846E-2</v>
+        <v>1.3888888888888895E-2</v>
       </c>
       <c r="Q3" t="s">
         <v>508</v>
@@ -24557,19 +24586,21 @@
     </row>
     <row r="4" spans="1:17">
       <c r="A4" s="99"/>
-      <c r="B4" s="80"/>
+      <c r="B4" s="80" t="s">
+        <v>528</v>
+      </c>
       <c r="C4" s="80" t="s">
-        <v>504</v>
+        <v>513</v>
       </c>
       <c r="D4" s="81">
-        <v>0.45833333333333331</v>
+        <v>0.39583333333333331</v>
       </c>
       <c r="E4" s="81">
         <v>0.47222222222222227</v>
       </c>
       <c r="F4" s="81">
         <f>E4-D4</f>
-        <v>1.3888888888888951E-2</v>
+        <v>7.6388888888888951E-2</v>
       </c>
       <c r="H4" s="83" t="s">
         <v>508</v>
@@ -24630,7 +24661,7 @@
       </c>
       <c r="I6" s="81">
         <f>SUMIFS(F2:F16, C2:C16,H6)</f>
-        <v>0</v>
+        <v>7.6388888888888951E-2</v>
       </c>
       <c r="Q6" t="s">
         <v>512</v>
@@ -24690,7 +24721,7 @@
     <row r="9" spans="1:17">
       <c r="A9" s="99"/>
       <c r="B9" s="80" t="s">
-        <v>764</v>
+        <v>766</v>
       </c>
       <c r="C9" s="80" t="s">
         <v>510</v>
@@ -24710,7 +24741,7 @@
       </c>
       <c r="I9" s="79">
         <f>SUM(I3:I8)</f>
-        <v>0.21527777777777773</v>
+        <v>0.27777777777777773</v>
       </c>
     </row>
     <row r="10" spans="1:17">
@@ -25074,7 +25105,7 @@
     <row r="34" spans="1:9">
       <c r="A34" s="99"/>
       <c r="B34" s="80" t="s">
-        <v>765</v>
+        <v>767</v>
       </c>
       <c r="C34" s="80" t="s">
         <v>504</v>
@@ -25126,7 +25157,7 @@
     <row r="36" spans="1:9">
       <c r="A36" s="99"/>
       <c r="B36" s="80" t="s">
-        <v>766</v>
+        <v>768</v>
       </c>
       <c r="C36" s="80" t="s">
         <v>508</v>
@@ -25152,7 +25183,7 @@
     <row r="37" spans="1:9">
       <c r="A37" s="99"/>
       <c r="B37" s="80" t="s">
-        <v>767</v>
+        <v>769</v>
       </c>
       <c r="C37" s="80" t="s">
         <v>510</v>
@@ -25178,7 +25209,7 @@
     <row r="38" spans="1:9">
       <c r="A38" s="99"/>
       <c r="B38" s="80" t="s">
-        <v>764</v>
+        <v>766</v>
       </c>
       <c r="C38" s="80" t="s">
         <v>510</v>
@@ -25354,7 +25385,7 @@
     <row r="49" spans="1:9">
       <c r="A49" s="99"/>
       <c r="B49" s="80" t="s">
-        <v>768</v>
+        <v>770</v>
       </c>
       <c r="C49" s="80" t="s">
         <v>504</v>
@@ -25406,7 +25437,7 @@
     <row r="51" spans="1:9">
       <c r="A51" s="99"/>
       <c r="B51" s="80" t="s">
-        <v>769</v>
+        <v>771</v>
       </c>
       <c r="C51" s="80" t="s">
         <v>504</v>
@@ -25458,7 +25489,7 @@
     <row r="53" spans="1:9">
       <c r="A53" s="99"/>
       <c r="B53" s="80" t="s">
-        <v>770</v>
+        <v>772</v>
       </c>
       <c r="C53" s="80" t="s">
         <v>504</v>
@@ -25510,7 +25541,7 @@
     <row r="55" spans="1:9">
       <c r="A55" s="99"/>
       <c r="B55" s="80" t="s">
-        <v>764</v>
+        <v>766</v>
       </c>
       <c r="C55" s="80" t="s">
         <v>510</v>
@@ -25530,7 +25561,7 @@
     <row r="56" spans="1:9">
       <c r="A56" s="99"/>
       <c r="B56" s="80" t="s">
-        <v>771</v>
+        <v>773</v>
       </c>
       <c r="C56" s="80" t="s">
         <v>504</v>
@@ -25550,7 +25581,7 @@
     <row r="57" spans="1:9">
       <c r="A57" s="99"/>
       <c r="B57" s="80" t="s">
-        <v>769</v>
+        <v>771</v>
       </c>
       <c r="C57" s="80" t="s">
         <v>504</v>
@@ -25944,7 +25975,7 @@
     <row r="79" spans="1:9">
       <c r="A79" s="99"/>
       <c r="B79" s="80" t="s">
-        <v>768</v>
+        <v>770</v>
       </c>
       <c r="C79" s="80" t="s">
         <v>504</v>
@@ -26074,7 +26105,7 @@
     <row r="84" spans="1:9">
       <c r="A84" s="99"/>
       <c r="B84" s="80" t="s">
-        <v>578</v>
+        <v>774</v>
       </c>
       <c r="C84" s="80" t="s">
         <v>504</v>
@@ -26439,7 +26470,7 @@
     <row r="108" spans="1:9">
       <c r="A108" s="99"/>
       <c r="B108" s="80" t="s">
-        <v>772</v>
+        <v>775</v>
       </c>
       <c r="C108" s="80" t="s">
         <v>116</v>
@@ -26465,7 +26496,7 @@
     <row r="109" spans="1:9">
       <c r="A109" s="99"/>
       <c r="B109" s="80" t="s">
-        <v>773</v>
+        <v>776</v>
       </c>
       <c r="C109" s="80" t="s">
         <v>516</v>
@@ -26491,7 +26522,7 @@
     <row r="110" spans="1:9">
       <c r="A110" s="99"/>
       <c r="B110" s="80" t="s">
-        <v>774</v>
+        <v>777</v>
       </c>
       <c r="C110" s="80" t="s">
         <v>504</v>
@@ -26517,7 +26548,7 @@
     <row r="111" spans="1:9">
       <c r="A111" s="99"/>
       <c r="B111" s="80" t="s">
-        <v>774</v>
+        <v>777</v>
       </c>
       <c r="C111" s="80" t="s">
         <v>504</v>
@@ -26569,7 +26600,7 @@
     <row r="113" spans="1:9">
       <c r="A113" s="99"/>
       <c r="B113" s="80" t="s">
-        <v>774</v>
+        <v>777</v>
       </c>
       <c r="C113" s="80" t="s">
         <v>504</v>
@@ -26595,7 +26626,7 @@
     <row r="114" spans="1:9">
       <c r="A114" s="99"/>
       <c r="B114" s="80" t="s">
-        <v>775</v>
+        <v>778</v>
       </c>
       <c r="C114" s="80" t="s">
         <v>510</v>
@@ -26621,7 +26652,7 @@
     <row r="115" spans="1:9">
       <c r="A115" s="99"/>
       <c r="B115" s="80" t="s">
-        <v>774</v>
+        <v>777</v>
       </c>
       <c r="C115" s="80" t="s">
         <v>504</v>
@@ -26710,7 +26741,7 @@
         <v>22</v>
       </c>
       <c r="B122" s="80" t="s">
-        <v>776</v>
+        <v>779</v>
       </c>
       <c r="C122" s="80" t="s">
         <v>508</v>
@@ -26761,7 +26792,7 @@
     <row r="124" spans="1:9">
       <c r="A124" s="99"/>
       <c r="B124" s="80" t="s">
-        <v>777</v>
+        <v>780</v>
       </c>
       <c r="C124" s="80" t="s">
         <v>504</v>
@@ -26837,7 +26868,7 @@
     <row r="127" spans="1:9">
       <c r="A127" s="99"/>
       <c r="B127" s="80" t="s">
-        <v>778</v>
+        <v>781</v>
       </c>
       <c r="C127" s="80" t="s">
         <v>510</v>
@@ -26863,7 +26894,7 @@
     <row r="128" spans="1:9">
       <c r="A128" s="99"/>
       <c r="B128" s="80" t="s">
-        <v>779</v>
+        <v>782</v>
       </c>
       <c r="C128" s="80" t="s">
         <v>504</v>
@@ -26915,7 +26946,7 @@
     <row r="130" spans="1:9">
       <c r="A130" s="99"/>
       <c r="B130" s="80" t="s">
-        <v>780</v>
+        <v>783</v>
       </c>
       <c r="C130" s="80" t="s">
         <v>504</v>
@@ -26955,7 +26986,7 @@
     <row r="132" spans="1:9">
       <c r="A132" s="99"/>
       <c r="B132" s="80" t="s">
-        <v>764</v>
+        <v>766</v>
       </c>
       <c r="C132" s="80" t="s">
         <v>510</v>
@@ -26974,7 +27005,7 @@
     <row r="133" spans="1:9">
       <c r="A133" s="99"/>
       <c r="B133" s="80" t="s">
-        <v>781</v>
+        <v>784</v>
       </c>
       <c r="C133" s="80" t="s">
         <v>504</v>
@@ -27053,7 +27084,7 @@
     <row r="138" spans="1:9">
       <c r="A138" s="99"/>
       <c r="B138" s="80" t="s">
-        <v>782</v>
+        <v>785</v>
       </c>
       <c r="C138" s="80" t="s">
         <v>510</v>
@@ -27105,7 +27136,7 @@
     <row r="140" spans="1:9">
       <c r="A140" s="99"/>
       <c r="B140" s="80" t="s">
-        <v>783</v>
+        <v>786</v>
       </c>
       <c r="C140" s="80" t="s">
         <v>504</v>
@@ -27157,7 +27188,7 @@
     <row r="142" spans="1:9">
       <c r="A142" s="99"/>
       <c r="B142" s="80" t="s">
-        <v>784</v>
+        <v>787</v>
       </c>
       <c r="C142" s="80" t="s">
         <v>504</v>
@@ -27209,7 +27240,7 @@
     <row r="144" spans="1:9">
       <c r="A144" s="99"/>
       <c r="B144" s="80" t="s">
-        <v>764</v>
+        <v>766</v>
       </c>
       <c r="C144" s="80" t="s">
         <v>510</v>
@@ -27235,7 +27266,7 @@
     <row r="145" spans="1:9">
       <c r="A145" s="99"/>
       <c r="B145" s="80" t="s">
-        <v>785</v>
+        <v>788</v>
       </c>
       <c r="C145" s="80" t="s">
         <v>504</v>
@@ -27255,7 +27286,7 @@
     <row r="146" spans="1:9">
       <c r="A146" s="99"/>
       <c r="B146" s="80" t="s">
-        <v>786</v>
+        <v>789</v>
       </c>
       <c r="C146" s="80" t="s">
         <v>510</v>
@@ -27383,7 +27414,7 @@
     <row r="154" spans="1:9">
       <c r="A154" s="99"/>
       <c r="B154" s="80" t="s">
-        <v>787</v>
+        <v>790</v>
       </c>
       <c r="C154" s="80" t="s">
         <v>504</v>
@@ -27409,7 +27440,7 @@
     <row r="155" spans="1:9">
       <c r="A155" s="99"/>
       <c r="B155" s="80" t="s">
-        <v>788</v>
+        <v>791</v>
       </c>
       <c r="C155" s="80" t="s">
         <v>504</v>
@@ -27513,7 +27544,7 @@
     <row r="159" spans="1:9">
       <c r="A159" s="99"/>
       <c r="B159" s="80" t="s">
-        <v>764</v>
+        <v>766</v>
       </c>
       <c r="C159" s="80" t="s">
         <v>510</v>
@@ -27778,7 +27809,7 @@
     <row r="3" spans="1:17">
       <c r="A3" s="99"/>
       <c r="B3" s="80" t="s">
-        <v>789</v>
+        <v>792</v>
       </c>
       <c r="C3" s="80" t="s">
         <v>504</v>
@@ -27798,7 +27829,7 @@
       </c>
       <c r="I3" s="81">
         <f>SUMIFS(F2:F16, C2:C16,H3)</f>
-        <v>4.8611111111111049E-2</v>
+        <v>8.6805555555555469E-2</v>
       </c>
       <c r="K3" t="s">
         <v>632</v>
@@ -27810,7 +27841,7 @@
     <row r="4" spans="1:17">
       <c r="A4" s="99"/>
       <c r="B4" s="80" t="s">
-        <v>790</v>
+        <v>793</v>
       </c>
       <c r="C4" s="80" t="s">
         <v>504</v>
@@ -27833,7 +27864,7 @@
         <v>6.9444444444444198E-3</v>
       </c>
       <c r="K4" t="s">
-        <v>791</v>
+        <v>794</v>
       </c>
       <c r="Q4" t="s">
         <v>510</v>
@@ -27847,18 +27878,22 @@
       <c r="C5" s="80" t="s">
         <v>516</v>
       </c>
-      <c r="D5" s="81"/>
-      <c r="E5" s="81"/>
+      <c r="D5" s="81">
+        <v>0.43402777777777773</v>
+      </c>
+      <c r="E5" s="81">
+        <v>0.44097222222222227</v>
+      </c>
       <c r="F5" s="81">
         <f>E5-D5</f>
-        <v>0</v>
+        <v>6.9444444444445308E-3</v>
       </c>
       <c r="H5" s="83" t="s">
         <v>510</v>
       </c>
       <c r="I5" s="81">
         <f>SUMIFS(F2:F16, C2:C16,H5)</f>
-        <v>0</v>
+        <v>4.1666666666666685E-2</v>
       </c>
       <c r="Q5" t="s">
         <v>513</v>
@@ -27867,14 +27902,20 @@
     <row r="6" spans="1:17">
       <c r="A6" s="99"/>
       <c r="B6" s="80" t="s">
-        <v>792</v>
-      </c>
-      <c r="C6" s="80"/>
-      <c r="D6" s="81"/>
-      <c r="E6" s="81"/>
+        <v>795</v>
+      </c>
+      <c r="C6" s="80" t="s">
+        <v>504</v>
+      </c>
+      <c r="D6" s="81">
+        <v>0.44097222222222227</v>
+      </c>
+      <c r="E6" s="81">
+        <v>0.47916666666666669</v>
+      </c>
       <c r="F6" s="81">
         <f>E6-D6</f>
-        <v>0</v>
+        <v>3.819444444444442E-2</v>
       </c>
       <c r="H6" s="83" t="s">
         <v>513</v>
@@ -27889,13 +27930,21 @@
     </row>
     <row r="7" spans="1:17">
       <c r="A7" s="99"/>
-      <c r="B7" s="80"/>
-      <c r="C7" s="80"/>
-      <c r="D7" s="81"/>
-      <c r="E7" s="81"/>
+      <c r="B7" s="80" t="s">
+        <v>766</v>
+      </c>
+      <c r="C7" s="80" t="s">
+        <v>510</v>
+      </c>
+      <c r="D7" s="81">
+        <v>0.47916666666666669</v>
+      </c>
+      <c r="E7" s="81">
+        <v>0.52083333333333337</v>
+      </c>
       <c r="F7" s="81">
         <f>E7-D7</f>
-        <v>0</v>
+        <v>4.1666666666666685E-2</v>
       </c>
       <c r="H7" s="83" t="s">
         <v>512</v>
@@ -27910,20 +27959,28 @@
     </row>
     <row r="8" spans="1:17">
       <c r="A8" s="99"/>
-      <c r="B8" s="80"/>
-      <c r="C8" s="80"/>
-      <c r="D8" s="81"/>
-      <c r="E8" s="81"/>
+      <c r="B8" s="80" t="s">
+        <v>518</v>
+      </c>
+      <c r="C8" s="80" t="s">
+        <v>516</v>
+      </c>
+      <c r="D8" s="81">
+        <v>0.52083333333333337</v>
+      </c>
+      <c r="E8" s="81">
+        <v>0.5625</v>
+      </c>
       <c r="F8" s="81">
         <f>E8-D8</f>
-        <v>0</v>
+        <v>4.166666666666663E-2</v>
       </c>
       <c r="H8" s="83" t="s">
         <v>516</v>
       </c>
       <c r="I8" s="81">
         <f>SUMIFS(F2:F16, C2:C16,H8)</f>
-        <v>0</v>
+        <v>4.861111111111116E-2</v>
       </c>
     </row>
     <row r="9" spans="1:17">
@@ -27941,7 +27998,7 @@
       </c>
       <c r="I9" s="79">
         <f>SUM(I3:I8)</f>
-        <v>5.5555555555555469E-2</v>
+        <v>0.18402777777777773</v>
       </c>
     </row>
     <row r="10" spans="1:17">
@@ -28028,7 +28085,7 @@
         <v>9</v>
       </c>
       <c r="B17" t="s">
-        <v>793</v>
+        <v>796</v>
       </c>
       <c r="C17" s="80" t="s">
         <v>510</v>
@@ -28079,13 +28136,13 @@
         <v>0.22222222222222227</v>
       </c>
       <c r="K18" t="s">
-        <v>794</v>
+        <v>797</v>
       </c>
     </row>
     <row r="19" spans="1:11">
       <c r="A19" s="99"/>
       <c r="B19" s="80" t="s">
-        <v>795</v>
+        <v>798</v>
       </c>
       <c r="C19" s="80" t="s">
         <v>504</v>
@@ -28137,7 +28194,7 @@
     <row r="21" spans="1:11">
       <c r="A21" s="99"/>
       <c r="B21" s="80" t="s">
-        <v>796</v>
+        <v>799</v>
       </c>
       <c r="C21" s="80" t="s">
         <v>504</v>
@@ -28163,7 +28220,7 @@
     <row r="22" spans="1:11">
       <c r="A22" s="99"/>
       <c r="B22" s="80" t="s">
-        <v>797</v>
+        <v>800</v>
       </c>
       <c r="C22" s="80" t="s">
         <v>510</v>
@@ -28215,7 +28272,7 @@
     <row r="24" spans="1:11">
       <c r="A24" s="99"/>
       <c r="B24" s="80" t="s">
-        <v>798</v>
+        <v>801</v>
       </c>
       <c r="C24" s="80" t="s">
         <v>504</v>
@@ -28241,7 +28298,7 @@
     <row r="25" spans="1:11">
       <c r="A25" s="99"/>
       <c r="B25" s="80" t="s">
-        <v>799</v>
+        <v>802</v>
       </c>
       <c r="C25" s="80" t="s">
         <v>504</v>
@@ -28281,7 +28338,7 @@
     <row r="27" spans="1:11">
       <c r="A27" s="99"/>
       <c r="B27" s="80" t="s">
-        <v>800</v>
+        <v>803</v>
       </c>
       <c r="C27" s="80" t="s">
         <v>504</v>
@@ -28371,7 +28428,7 @@
     <row r="33" spans="1:11">
       <c r="A33" s="99"/>
       <c r="B33" s="80" t="s">
-        <v>790</v>
+        <v>793</v>
       </c>
       <c r="C33" s="80" t="s">
         <v>513</v>
@@ -28397,7 +28454,7 @@
     <row r="34" spans="1:11">
       <c r="A34" s="99"/>
       <c r="B34" s="18" t="s">
-        <v>801</v>
+        <v>804</v>
       </c>
       <c r="C34" s="80" t="s">
         <v>504</v>
@@ -28449,7 +28506,7 @@
     <row r="36" spans="1:11">
       <c r="A36" s="99"/>
       <c r="B36" s="80" t="s">
-        <v>764</v>
+        <v>766</v>
       </c>
       <c r="C36" s="80" t="s">
         <v>510</v>
@@ -28478,7 +28535,7 @@
     <row r="37" spans="1:11">
       <c r="A37" s="99"/>
       <c r="B37" s="80" t="s">
-        <v>802</v>
+        <v>805</v>
       </c>
       <c r="C37" s="80" t="s">
         <v>508</v>
@@ -28501,7 +28558,7 @@
         <v>0</v>
       </c>
       <c r="K37" s="80" t="s">
-        <v>803</v>
+        <v>806</v>
       </c>
     </row>
     <row r="38" spans="1:11">
@@ -28533,7 +28590,7 @@
     <row r="39" spans="1:11">
       <c r="A39" s="99"/>
       <c r="B39" s="18" t="s">
-        <v>804</v>
+        <v>807</v>
       </c>
       <c r="C39" s="80" t="s">
         <v>504</v>
@@ -28559,7 +28616,7 @@
     <row r="40" spans="1:11">
       <c r="A40" s="99"/>
       <c r="B40" s="80" t="s">
-        <v>805</v>
+        <v>808</v>
       </c>
       <c r="C40" s="80" t="s">
         <v>504</v>
@@ -28579,7 +28636,7 @@
     <row r="41" spans="1:11">
       <c r="A41" s="99"/>
       <c r="B41" s="80" t="s">
-        <v>806</v>
+        <v>809</v>
       </c>
       <c r="C41" s="80" t="s">
         <v>510</v>
@@ -28707,13 +28764,13 @@
         <v>0.26736111111111088</v>
       </c>
       <c r="K48" t="s">
-        <v>807</v>
+        <v>810</v>
       </c>
     </row>
     <row r="49" spans="1:11">
       <c r="A49" s="99"/>
       <c r="B49" s="80" t="s">
-        <v>808</v>
+        <v>811</v>
       </c>
       <c r="C49" s="80" t="s">
         <v>504</v>
@@ -28736,7 +28793,7 @@
         <v>1.3888888888888895E-2</v>
       </c>
       <c r="K49" t="s">
-        <v>809</v>
+        <v>812</v>
       </c>
     </row>
     <row r="50" spans="1:11">
@@ -28768,7 +28825,7 @@
     <row r="51" spans="1:11">
       <c r="A51" s="99"/>
       <c r="B51" s="80" t="s">
-        <v>810</v>
+        <v>813</v>
       </c>
       <c r="C51" s="80" t="s">
         <v>504</v>
@@ -28794,7 +28851,7 @@
     <row r="52" spans="1:11">
       <c r="A52" s="99"/>
       <c r="B52" s="80" t="s">
-        <v>811</v>
+        <v>814</v>
       </c>
       <c r="C52" s="80" t="s">
         <v>510</v>
@@ -28846,7 +28903,7 @@
     <row r="54" spans="1:11">
       <c r="A54" s="99"/>
       <c r="B54" s="80" t="s">
-        <v>812</v>
+        <v>815</v>
       </c>
       <c r="C54" s="80" t="s">
         <v>504</v>
@@ -28892,7 +28949,7 @@
     <row r="56" spans="1:11">
       <c r="A56" s="99"/>
       <c r="B56" s="80" t="s">
-        <v>813</v>
+        <v>816</v>
       </c>
       <c r="C56" s="80" t="s">
         <v>504</v>
@@ -28912,7 +28969,7 @@
     <row r="57" spans="1:11">
       <c r="A57" s="99"/>
       <c r="B57" s="80" t="s">
-        <v>814</v>
+        <v>817</v>
       </c>
       <c r="C57" s="80" t="s">
         <v>504</v>
@@ -29034,7 +29091,7 @@
     <row r="64" spans="1:11">
       <c r="A64" s="99"/>
       <c r="B64" s="80" t="s">
-        <v>815</v>
+        <v>818</v>
       </c>
       <c r="C64" s="80" t="s">
         <v>504</v>
@@ -29057,13 +29114,13 @@
         <v>1.3888888888888895E-2</v>
       </c>
       <c r="K64" t="s">
-        <v>816</v>
+        <v>819</v>
       </c>
     </row>
     <row r="65" spans="1:11">
       <c r="A65" s="99"/>
       <c r="B65" s="80" t="s">
-        <v>773</v>
+        <v>776</v>
       </c>
       <c r="C65" s="80" t="s">
         <v>516</v>
@@ -29089,7 +29146,7 @@
     <row r="66" spans="1:11">
       <c r="A66" s="99"/>
       <c r="B66" t="s">
-        <v>817</v>
+        <v>820</v>
       </c>
       <c r="C66" s="80" t="s">
         <v>504</v>
@@ -29115,7 +29172,7 @@
     <row r="67" spans="1:11">
       <c r="A67" s="99"/>
       <c r="B67" s="80" t="s">
-        <v>818</v>
+        <v>821</v>
       </c>
       <c r="C67" s="80" t="s">
         <v>510</v>
@@ -29167,7 +29224,7 @@
     <row r="69" spans="1:11">
       <c r="A69" s="99"/>
       <c r="B69" s="80" t="s">
-        <v>819</v>
+        <v>822</v>
       </c>
       <c r="C69" s="80" t="s">
         <v>504</v>
@@ -29193,7 +29250,7 @@
     <row r="70" spans="1:11">
       <c r="A70" s="99"/>
       <c r="B70" t="s">
-        <v>820</v>
+        <v>823</v>
       </c>
       <c r="C70" s="80" t="s">
         <v>504</v>
@@ -29213,7 +29270,7 @@
     <row r="71" spans="1:11">
       <c r="A71" s="99"/>
       <c r="B71" s="80" t="s">
-        <v>821</v>
+        <v>824</v>
       </c>
       <c r="C71" s="80" t="s">
         <v>516</v>
@@ -29233,7 +29290,7 @@
     <row r="72" spans="1:11">
       <c r="A72" s="99"/>
       <c r="B72" s="80" t="s">
-        <v>822</v>
+        <v>825</v>
       </c>
       <c r="C72" s="80" t="s">
         <v>504</v>
@@ -29252,7 +29309,7 @@
     <row r="73" spans="1:11">
       <c r="A73" s="99"/>
       <c r="B73" s="80" t="s">
-        <v>823</v>
+        <v>826</v>
       </c>
       <c r="C73" s="80" t="s">
         <v>510</v>
@@ -29357,7 +29414,7 @@
     <row r="79" spans="1:11">
       <c r="A79" s="99"/>
       <c r="B79" s="80" t="s">
-        <v>824</v>
+        <v>827</v>
       </c>
       <c r="C79" s="80" t="s">
         <v>504</v>
@@ -29406,13 +29463,13 @@
         <v>9.0277777777777735E-2</v>
       </c>
       <c r="K80" t="s">
-        <v>825</v>
+        <v>828</v>
       </c>
     </row>
     <row r="81" spans="1:11">
       <c r="A81" s="99"/>
       <c r="B81" s="80" t="s">
-        <v>826</v>
+        <v>829</v>
       </c>
       <c r="C81" s="80" t="s">
         <v>504</v>
@@ -29435,13 +29492,13 @@
         <v>2.083333333333337E-2</v>
       </c>
       <c r="K81" t="s">
-        <v>827</v>
+        <v>830</v>
       </c>
     </row>
     <row r="82" spans="1:11">
       <c r="A82" s="99"/>
       <c r="B82" s="80" t="s">
-        <v>828</v>
+        <v>831</v>
       </c>
       <c r="C82" s="80" t="s">
         <v>510</v>
@@ -29493,7 +29550,7 @@
     <row r="84" spans="1:11">
       <c r="A84" s="99"/>
       <c r="B84" s="80" t="s">
-        <v>829</v>
+        <v>832</v>
       </c>
       <c r="C84" s="80" t="s">
         <v>504</v>
@@ -29539,7 +29596,7 @@
     <row r="86" spans="1:11">
       <c r="A86" s="99"/>
       <c r="B86" s="80" t="s">
-        <v>826</v>
+        <v>829</v>
       </c>
       <c r="C86" s="80" t="s">
         <v>504</v>
@@ -29559,7 +29616,7 @@
     <row r="87" spans="1:11">
       <c r="A87" s="99"/>
       <c r="B87" s="80" t="s">
-        <v>830</v>
+        <v>833</v>
       </c>
       <c r="C87" s="80" t="s">
         <v>510</v>
@@ -29621,7 +29678,7 @@
     </row>
     <row r="92" spans="1:11">
       <c r="A92" s="99" t="s">
-        <v>831</v>
+        <v>834</v>
       </c>
       <c r="B92" s="80" t="s">
         <v>572</v>
@@ -29649,7 +29706,7 @@
     <row r="93" spans="1:11">
       <c r="A93" s="99"/>
       <c r="B93" s="80" t="s">
-        <v>832</v>
+        <v>835</v>
       </c>
       <c r="C93" s="80" t="s">
         <v>504</v>
@@ -29735,7 +29792,7 @@
     <row r="96" spans="1:11">
       <c r="A96" s="99"/>
       <c r="B96" s="80" t="s">
-        <v>775</v>
+        <v>778</v>
       </c>
       <c r="C96" s="80" t="s">
         <v>510</v>
@@ -29787,7 +29844,7 @@
     <row r="98" spans="1:9">
       <c r="A98" s="99"/>
       <c r="B98" s="80" t="s">
-        <v>833</v>
+        <v>836</v>
       </c>
       <c r="C98" s="80" t="s">
         <v>504</v>
@@ -29839,7 +29896,7 @@
     <row r="100" spans="1:9">
       <c r="A100" s="99"/>
       <c r="B100" s="80" t="s">
-        <v>834</v>
+        <v>837</v>
       </c>
       <c r="C100" s="80" t="s">
         <v>504</v>
@@ -29859,7 +29916,7 @@
     <row r="101" spans="1:9">
       <c r="A101" s="99"/>
       <c r="B101" s="80" t="s">
-        <v>835</v>
+        <v>838</v>
       </c>
       <c r="C101" s="80" t="s">
         <v>504</v>
@@ -29961,7 +30018,7 @@
     <row r="108" spans="1:9">
       <c r="A108" s="99"/>
       <c r="B108" s="80" t="s">
-        <v>836</v>
+        <v>839</v>
       </c>
       <c r="C108" s="80" t="s">
         <v>504</v>
@@ -29987,7 +30044,7 @@
     <row r="109" spans="1:9">
       <c r="A109" s="99"/>
       <c r="B109" s="80" t="s">
-        <v>773</v>
+        <v>776</v>
       </c>
       <c r="C109" s="80" t="s">
         <v>516</v>
@@ -30013,7 +30070,7 @@
     <row r="110" spans="1:9">
       <c r="A110" s="99"/>
       <c r="B110" s="80" t="s">
-        <v>837</v>
+        <v>840</v>
       </c>
       <c r="C110" s="80" t="s">
         <v>510</v>
@@ -30039,7 +30096,7 @@
     <row r="111" spans="1:9">
       <c r="A111" s="99"/>
       <c r="B111" s="80" t="s">
-        <v>775</v>
+        <v>778</v>
       </c>
       <c r="C111" s="80" t="s">
         <v>510</v>
@@ -30091,7 +30148,7 @@
     <row r="113" spans="1:9">
       <c r="A113" s="99"/>
       <c r="B113" s="80" t="s">
-        <v>838</v>
+        <v>841</v>
       </c>
       <c r="C113" s="80" t="s">
         <v>504</v>
@@ -30117,7 +30174,7 @@
     <row r="114" spans="1:9">
       <c r="A114" s="99"/>
       <c r="B114" s="80" t="s">
-        <v>839</v>
+        <v>842</v>
       </c>
       <c r="C114" s="80" t="s">
         <v>504</v>
@@ -30163,7 +30220,7 @@
     <row r="116" spans="1:9">
       <c r="A116" s="99"/>
       <c r="B116" s="80" t="s">
-        <v>839</v>
+        <v>842</v>
       </c>
       <c r="C116" s="80" t="s">
         <v>504</v>
@@ -30183,7 +30240,7 @@
     <row r="117" spans="1:9">
       <c r="A117" s="99"/>
       <c r="B117" s="80" t="s">
-        <v>839</v>
+        <v>842</v>
       </c>
       <c r="C117" s="80" t="s">
         <v>504</v>
@@ -30248,7 +30305,7 @@
         <v>22</v>
       </c>
       <c r="B122" s="80" t="s">
-        <v>840</v>
+        <v>843</v>
       </c>
       <c r="C122" s="80" t="s">
         <v>508</v>
@@ -30299,7 +30356,7 @@
     <row r="124" spans="1:9">
       <c r="A124" s="99"/>
       <c r="B124" s="80" t="s">
-        <v>841</v>
+        <v>844</v>
       </c>
       <c r="C124" s="80" t="s">
         <v>504</v>
@@ -30351,7 +30408,7 @@
     <row r="126" spans="1:9">
       <c r="A126" s="99"/>
       <c r="B126" s="80" t="s">
-        <v>842</v>
+        <v>845</v>
       </c>
       <c r="C126" s="80" t="s">
         <v>504</v>
@@ -30377,7 +30434,7 @@
     <row r="127" spans="1:9">
       <c r="A127" s="99"/>
       <c r="B127" s="80" t="s">
-        <v>843</v>
+        <v>846</v>
       </c>
       <c r="C127" s="80" t="s">
         <v>510</v>
@@ -30429,7 +30486,7 @@
     <row r="129" spans="1:9">
       <c r="A129" s="99"/>
       <c r="B129" s="80" t="s">
-        <v>844</v>
+        <v>847</v>
       </c>
       <c r="C129" s="80" t="s">
         <v>504</v>
@@ -30475,7 +30532,7 @@
     <row r="131" spans="1:9">
       <c r="A131" s="99"/>
       <c r="B131" s="80" t="s">
-        <v>845</v>
+        <v>848</v>
       </c>
       <c r="C131" s="80" t="s">
         <v>504</v>
@@ -30495,7 +30552,7 @@
     <row r="132" spans="1:9">
       <c r="A132" s="99"/>
       <c r="B132" s="80" t="s">
-        <v>846</v>
+        <v>849</v>
       </c>
       <c r="C132" s="80" t="s">
         <v>504</v>
@@ -30560,7 +30617,7 @@
         <v>647</v>
       </c>
       <c r="B137" s="80" t="s">
-        <v>840</v>
+        <v>843</v>
       </c>
       <c r="C137" s="80" t="s">
         <v>508</v>
@@ -30611,7 +30668,7 @@
     <row r="139" spans="1:9">
       <c r="A139" s="99"/>
       <c r="B139" s="80" t="s">
-        <v>847</v>
+        <v>850</v>
       </c>
       <c r="C139" s="80" t="s">
         <v>504</v>
@@ -30663,7 +30720,7 @@
     <row r="141" spans="1:9">
       <c r="A141" s="99"/>
       <c r="B141" s="80" t="s">
-        <v>848</v>
+        <v>851</v>
       </c>
       <c r="C141" s="80" t="s">
         <v>510</v>
@@ -30715,7 +30772,7 @@
     <row r="143" spans="1:9">
       <c r="A143" s="99"/>
       <c r="B143" s="80" t="s">
-        <v>849</v>
+        <v>852</v>
       </c>
       <c r="C143" s="80" t="s">
         <v>510</v>
@@ -30741,7 +30798,7 @@
     <row r="144" spans="1:9">
       <c r="A144" s="99"/>
       <c r="B144" s="80" t="s">
-        <v>850</v>
+        <v>853</v>
       </c>
       <c r="C144" s="80" t="s">
         <v>504</v>
@@ -30787,7 +30844,7 @@
     <row r="146" spans="1:9">
       <c r="A146" s="99"/>
       <c r="B146" s="80" t="s">
-        <v>851</v>
+        <v>854</v>
       </c>
       <c r="C146" s="80" t="s">
         <v>504</v>
@@ -30915,7 +30972,7 @@
     <row r="154" spans="1:9">
       <c r="A154" s="99"/>
       <c r="B154" s="80" t="s">
-        <v>774</v>
+        <v>777</v>
       </c>
       <c r="C154" s="80" t="s">
         <v>504</v>
@@ -30941,7 +30998,7 @@
     <row r="155" spans="1:9">
       <c r="A155" s="99"/>
       <c r="B155" s="80" t="s">
-        <v>852</v>
+        <v>855</v>
       </c>
       <c r="C155" s="80" t="s">
         <v>510</v>
@@ -31045,7 +31102,7 @@
     <row r="159" spans="1:9">
       <c r="A159" s="99"/>
       <c r="B159" s="80" t="s">
-        <v>819</v>
+        <v>822</v>
       </c>
       <c r="C159" s="80" t="s">
         <v>504</v>
@@ -31071,7 +31128,7 @@
     <row r="160" spans="1:9">
       <c r="A160" s="99"/>
       <c r="B160" s="80" t="s">
-        <v>853</v>
+        <v>856</v>
       </c>
       <c r="C160" s="80" t="s">
         <v>504</v>
@@ -31091,7 +31148,7 @@
     <row r="161" spans="1:9">
       <c r="A161" s="99"/>
       <c r="B161" s="80" t="s">
-        <v>854</v>
+        <v>857</v>
       </c>
       <c r="C161" s="80" t="s">
         <v>504</v>
@@ -31111,7 +31168,7 @@
     <row r="162" spans="1:9">
       <c r="A162" s="99"/>
       <c r="B162" s="80" t="s">
-        <v>855</v>
+        <v>858</v>
       </c>
       <c r="C162" s="80" t="s">
         <v>504</v>

</xml_diff>